<commit_message>
Changed commands and tests
</commit_message>
<xml_diff>
--- a/TestSuiteReport.xlsx
+++ b/TestSuiteReport.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>ID</t>
   </si>
@@ -37,7 +37,7 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Jun-04-2022</t>
+    <t>Jun-05-2022</t>
   </si>
   <si>
     <t>U2</t>
@@ -64,16 +64,28 @@
     <t>U5</t>
   </si>
   <si>
+    <t>!play command - with no link input</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>!play command - with incorrect link</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
     <t>Queue another song while bot is playing music</t>
   </si>
   <si>
-    <t>U6</t>
+    <t>U8</t>
   </si>
   <si>
     <t>Using !skip command in text channel to skip music bot's current song</t>
   </si>
   <si>
-    <t>U7</t>
+    <t>U9</t>
   </si>
   <si>
     <t>Using !stop command in text channel to stop the music bot</t>
@@ -82,7 +94,7 @@
     <t>Passed / Total</t>
   </si>
   <si>
-    <t>6/7</t>
+    <t>8/9</t>
   </si>
 </sst>
 </file>
@@ -414,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,7 +510,7 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -526,18 +538,46 @@
         <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>